<commit_message>
Added hose bracket for lights
</commit_message>
<xml_diff>
--- a/CopyStand/BOM.xlsx
+++ b/CopyStand/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="45040" yWindow="0" windowWidth="25600" windowHeight="18400" tabRatio="500"/>
+    <workbookView xWindow="39100" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="72">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -205,6 +205,36 @@
   </si>
   <si>
     <t>1/4"-20 x 3/8" thumbscrew (pack of 10)</t>
+  </si>
+  <si>
+    <t>3/8" split lock washer (packs of 50)</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#94241a290/=11soufa</t>
+  </si>
+  <si>
+    <t>3/8"-16 socket cap screw (pack of 25)</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#92196a622/=11sossg</t>
+  </si>
+  <si>
+    <t>10-32 x 3/8" low-profile socket head cap screw (pack of 50)</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#90665a135/=11u6kcy</t>
+  </si>
+  <si>
+    <t>Loc-Line coolant hose (1/4" ID x 12")</t>
+  </si>
+  <si>
+    <t>Loc-Line threaded end connector (pack of 4)</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/mv1459440175/#10095K31</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#10095k42/=11u6mmr</t>
   </si>
 </sst>
 </file>
@@ -280,9 +310,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -395,7 +449,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="92">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -430,6 +484,18 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -463,6 +529,18 @@
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -792,7 +870,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -853,7 +931,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="E2" s="6">
-        <f t="shared" ref="E2:E12" si="1">D2*0.69</f>
+        <f t="shared" ref="E2:E17" si="1">D2*0.69</f>
         <v>7.0379999999999994</v>
       </c>
       <c r="F2" s="13" t="s">
@@ -1149,315 +1227,459 @@
         <v>57</v>
       </c>
     </row>
+    <row r="13" spans="1:8" ht="20" customHeight="1">
+      <c r="A13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="5">
+        <f>9.5/50</f>
+        <v>0.19</v>
+      </c>
+      <c r="C13" s="8">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5">
+        <f>C13*B13</f>
+        <v>9.5</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="1"/>
+        <v>6.5549999999999997</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="14" spans="1:8" ht="20" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="B14" s="5">
-        <v>22.42</v>
+        <f>11.09/25</f>
+        <v>0.44359999999999999</v>
       </c>
       <c r="C14" s="8">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5">
         <f>C14*B14</f>
-        <v>22.42</v>
+        <v>11.09</v>
       </c>
       <c r="E14" s="6">
-        <f>D14*0.69</f>
-        <v>15.469799999999999</v>
-      </c>
-      <c r="F14" s="13" t="s">
+        <f t="shared" si="1"/>
+        <v>7.652099999999999</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="20" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B15" s="5">
-        <v>12.95</v>
+        <f>6.24/50</f>
+        <v>0.12480000000000001</v>
       </c>
       <c r="C15" s="8">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D15" s="5">
         <f>C15*B15</f>
-        <v>12.95</v>
+        <v>6.24</v>
       </c>
       <c r="E15" s="6">
-        <f>D15*0.69</f>
-        <v>8.9354999999999993</v>
-      </c>
-      <c r="F15" s="13" t="s">
+        <f t="shared" si="1"/>
+        <v>4.3056000000000001</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="B16" s="5">
-        <v>17.88</v>
+        <v>6.59</v>
       </c>
       <c r="C16" s="8">
         <v>2</v>
       </c>
       <c r="D16" s="5">
         <f>C16*B16</f>
-        <v>35.76</v>
+        <v>13.18</v>
       </c>
       <c r="E16" s="6">
-        <f>D16*0.69</f>
-        <v>24.674399999999995</v>
-      </c>
-      <c r="F16" s="13" t="s">
+        <f t="shared" si="1"/>
+        <v>9.094199999999999</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B17" s="5">
-        <v>16.28</v>
+        <f>4.35/4</f>
+        <v>1.0874999999999999</v>
       </c>
       <c r="C17" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D17" s="5">
         <f>C17*B17</f>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="1"/>
+        <v>3.0014999999999996</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20" customHeight="1">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="5">
+        <v>22.42</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
+        <f>C19*B19</f>
+        <v>22.42</v>
+      </c>
+      <c r="E19" s="6">
+        <f>D19*0.69</f>
+        <v>15.469799999999999</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20" customHeight="1">
+      <c r="A20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="5">
+        <v>12.95</v>
+      </c>
+      <c r="C20" s="8">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <f>C20*B20</f>
+        <v>12.95</v>
+      </c>
+      <c r="E20" s="6">
+        <f>D20*0.69</f>
+        <v>8.9354999999999993</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="20" customHeight="1">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <v>17.88</v>
+      </c>
+      <c r="C21" s="8">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5">
+        <f>C21*B21</f>
+        <v>35.76</v>
+      </c>
+      <c r="E21" s="6">
+        <f>D21*0.69</f>
+        <v>24.674399999999995</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20" customHeight="1">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="5">
         <v>16.28</v>
       </c>
-      <c r="E17" s="6">
-        <f>D17*0.69</f>
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
+        <f>C22*B22</f>
+        <v>16.28</v>
+      </c>
+      <c r="E22" s="6">
+        <f>D22*0.69</f>
         <v>11.2332</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20" customHeight="1">
-      <c r="A19" s="7" t="s">
+    <row r="24" spans="1:8" ht="20" customHeight="1">
+      <c r="A24" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="2">
-        <f>SUM(D2:D17)</f>
-        <v>177.75000000000003</v>
-      </c>
-      <c r="E19" s="3">
-        <f>SUM(E2:E17)</f>
-        <v>122.64749999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="20" customHeight="1">
-      <c r="A31" s="1" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="2">
+        <f>SUM(D2:D22)</f>
+        <v>222.10999999999999</v>
+      </c>
+      <c r="E24" s="3">
+        <f>SUM(E2:E22)</f>
+        <v>153.25590000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="20" customHeight="1">
+      <c r="A33" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="20" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="5">
-        <v>4.3499999999999996</v>
-      </c>
-      <c r="C32" s="10">
-        <v>2</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="20" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="5">
-        <v>11.06</v>
-      </c>
-      <c r="C33" s="8">
-        <v>1</v>
-      </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1">
       <c r="A34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="5">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="C34" s="10">
+        <v>2</v>
+      </c>
+      <c r="F34" s="13"/>
+      <c r="G34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="20" customHeight="1">
+      <c r="A35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="5">
+        <v>11.06</v>
+      </c>
+      <c r="C35" s="8">
+        <v>1</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="20" customHeight="1">
+      <c r="A36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B36" s="5">
         <f>8.44/50</f>
         <v>0.16879999999999998</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C36" s="8">
         <v>50</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H34" s="4" t="s">
+      <c r="F36" s="13"/>
+      <c r="G36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="20" customHeight="1">
-      <c r="A36" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B36" s="5">
-        <v>10.8</v>
-      </c>
-      <c r="C36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="5">
-        <f>C36*B36</f>
-        <v>10.8</v>
-      </c>
-      <c r="E36" s="6">
-        <f>D36*0.69</f>
-        <v>7.452</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="20" customHeight="1">
-      <c r="A37" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="5">
-        <v>3.38</v>
-      </c>
-      <c r="C37" s="8">
-        <v>2</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B38" s="5">
-        <v>1.32</v>
+        <v>10.8</v>
       </c>
       <c r="C38" s="8">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D38" s="5">
+        <f>C38*B38</f>
+        <v>10.8</v>
+      </c>
+      <c r="E38" s="6">
+        <f>D38*0.69</f>
+        <v>7.452</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B39" s="5">
-        <v>2.13</v>
+        <v>3.38</v>
       </c>
       <c r="C39" s="8">
         <v>2</v>
       </c>
-      <c r="D39" s="5">
-        <f>C39*B39</f>
-        <v>4.26</v>
-      </c>
-      <c r="E39" s="6">
-        <f>D39*0.69</f>
-        <v>2.9393999999999996</v>
-      </c>
       <c r="G39" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="20" customHeight="1">
       <c r="A40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1.32</v>
+      </c>
+      <c r="C40" s="8">
+        <v>2</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="20" customHeight="1">
+      <c r="A41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="5">
+        <v>2.13</v>
+      </c>
+      <c r="C41" s="8">
+        <v>2</v>
+      </c>
+      <c r="D41" s="5">
+        <f>C41*B41</f>
+        <v>4.26</v>
+      </c>
+      <c r="E41" s="6">
+        <f>D41*0.69</f>
+        <v>2.9393999999999996</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="20" customHeight="1">
+      <c r="A42" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B42" s="5">
         <f>19.32/100</f>
         <v>0.19320000000000001</v>
       </c>
-      <c r="C40" s="8">
+      <c r="C42" s="8">
         <v>100</v>
       </c>
-      <c r="D40" s="5">
-        <f>C40*B40</f>
+      <c r="D42" s="5">
+        <f>C42*B42</f>
         <v>19.32</v>
       </c>
-      <c r="E40" s="6">
-        <f>D40*0.69</f>
+      <c r="E42" s="6">
+        <f>D42*0.69</f>
         <v>13.3308</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="20" customHeight="1">
-      <c r="A42" s="4" t="s">
+    <row r="44" spans="1:8" ht="20" customHeight="1">
+      <c r="A44" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B44" s="5">
         <f>8/10</f>
         <v>0.8</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C44" s="8">
         <v>10</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H42" s="4" t="s">
+      <c r="G44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="4" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>